<commit_message>
Adicionando Ferramenta Criada - Planilha
</commit_message>
<xml_diff>
--- a/Desafio - Ferramenta Financeira.xlsx
+++ b/Desafio - Ferramenta Financeira.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e03ba183db14d845/Cursos/Bootcamp Santander - Excel com Inteligência Artificial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="610" documentId="8_{CEAE5B7E-C13E-4338-AACE-AC5E83AF09C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD51C828-EC65-4CE1-B47D-BA3879654765}"/>
+  <xr:revisionPtr revIDLastSave="617" documentId="8_{CEAE5B7E-C13E-4338-AACE-AC5E83AF09C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8380AC7F-8721-43B7-97AE-6515892DD5C3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="0" xr2:uid="{483C08B3-EF63-4514-89F2-C2CDDD888BDA}"/>
   </bookViews>
@@ -158,8 +158,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000%"/>
-    <numFmt numFmtId="171" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -548,14 +548,8 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -563,163 +557,129 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="8"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="9" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="9" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="9" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="9" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="9" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="9" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="9" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="9" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="8"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="8"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="9" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="9" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="8"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="8"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -728,6 +688,42 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -787,6 +783,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-0489-421A-A37B-E382B7E49258}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -804,6 +805,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-0489-421A-A37B-E382B7E49258}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -821,6 +827,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-0489-421A-A37B-E382B7E49258}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -838,6 +849,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-0489-421A-A37B-E382B7E49258}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -855,6 +871,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-0489-421A-A37B-E382B7E49258}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -872,6 +893,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-0489-421A-A37B-E382B7E49258}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1004,6 +1030,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-0489-421A-A37B-E382B7E49258}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1021,6 +1052,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-0489-421A-A37B-E382B7E49258}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1038,6 +1074,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-0489-421A-A37B-E382B7E49258}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1055,6 +1096,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-0489-421A-A37B-E382B7E49258}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1072,6 +1118,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-0489-421A-A37B-E382B7E49258}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -1089,6 +1140,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-0489-421A-A37B-E382B7E49258}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1179,22 +1235,22 @@
                 <c:formatCode>"R$"\ #,##0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>250</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2430,8 +2486,8 @@
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" style="28" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" style="2" customWidth="1"/>
     <col min="4" max="4" width="19.44140625" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="13.44140625" hidden="1" customWidth="1"/>
@@ -2441,38 +2497,38 @@
   <sheetData>
     <row r="7" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="11"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="44"/>
     </row>
     <row r="9" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="60">
-        <v>3500</v>
+      <c r="C9" s="53"/>
+      <c r="D9" s="34">
+        <v>2000</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="61">
-        <v>6.0000000000000001E-3</v>
+      <c r="C10" s="55"/>
+      <c r="D10" s="35">
+        <v>0.01</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="14">
+      <c r="C11" s="57"/>
+      <c r="D11" s="6">
         <f>D9*30%</f>
-        <v>1050</v>
+        <v>600</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
@@ -2481,273 +2537,267 @@
     </row>
     <row r="13" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="2:4" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="2:4" s="3" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="29" t="s">
+      <c r="C14" s="46"/>
+      <c r="D14" s="47"/>
+    </row>
+    <row r="15" spans="2:4" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="15">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" s="3" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="31" t="s">
+      <c r="C15" s="59"/>
+      <c r="D15" s="7">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="3" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="31" t="s">
+      <c r="C16" s="61"/>
+      <c r="D16" s="8">
         <v>2</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="17">
+    </row>
+    <row r="17" spans="1:4" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="61"/>
+      <c r="D17" s="9">
         <f>Rendimento_Carteira</f>
-        <v>6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="3" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="33" t="s">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="18">
+      <c r="C18" s="39"/>
+      <c r="D18" s="10">
         <f>FV(tx_mensal,qtd_anos*12,Aporte*-1)</f>
-        <v>87501.504733170746</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="3" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="35" t="s">
+        <v>16184.078911914899</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="19">
+      <c r="C19" s="41"/>
+      <c r="D19" s="11">
         <f>patrimonio*tx_mensal</f>
-        <v>525.00902839902449</v>
+        <v>161.84078911914901</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:4" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9" t="s">
+      <c r="C22" s="51"/>
+      <c r="D22" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="7">
+      <c r="A23" s="4">
         <v>2</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="12">
         <f>FV($D$17,$A23*12,$D$15*-1)</f>
-        <v>12865.607682079208</v>
-      </c>
-      <c r="D23" s="21">
+        <v>16184.078911914899</v>
+      </c>
+      <c r="D23" s="13">
         <f>C23*tx_mensal</f>
-        <v>77.193646092475248</v>
+        <v>161.84078911914901</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="7">
+      <c r="A24" s="4">
         <v>5</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="14">
         <f>FV($D$17,$A24*12,$D$15*-1)</f>
-        <v>35982.367668429237</v>
-      </c>
-      <c r="D24" s="18">
+        <v>49001.801913845477</v>
+      </c>
+      <c r="D24" s="10">
         <f>C24*tx_mensal</f>
-        <v>215.89420601057543</v>
+        <v>490.01801913845475</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="7">
+      <c r="A25" s="4">
         <v>10</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="14">
         <f>FV($D$17,$A25*12,$D$15*-1)</f>
-        <v>87501.504733170746</v>
-      </c>
-      <c r="D25" s="18">
+        <v>138023.2136744202</v>
+      </c>
+      <c r="D25" s="10">
         <f>C25*tx_mensal</f>
-        <v>525.00902839902449</v>
+        <v>1380.2321367442021</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="7">
+      <c r="A26" s="4">
         <v>20</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="22">
+      <c r="C26" s="14">
         <f>FV($D$17,$A26*12,$D$15*-1)</f>
-        <v>266881.16943317064</v>
-      </c>
-      <c r="D26" s="18">
+        <v>593553.21923241776</v>
+      </c>
+      <c r="D26" s="10">
         <f>C26*tx_mensal</f>
-        <v>1601.2870165990239</v>
+        <v>5935.5321923241781</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="7">
+      <c r="A27" s="4">
         <v>30</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="23">
+      <c r="C27" s="15">
         <f>FV($D$17,$A27*12,$D$15*-1)</f>
-        <v>634612.72109054984</v>
-      </c>
-      <c r="D27" s="24">
+        <v>2096978.4796611038</v>
+      </c>
+      <c r="D27" s="16">
         <f>C27*tx_mensal</f>
-        <v>3807.6763265432992</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="4"/>
-      <c r="D28"/>
+        <v>20969.784796611038</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="49" t="s">
+      <c r="B30" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="62" t="s">
+      <c r="C30" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="63"/>
+      <c r="D30" s="49"/>
     </row>
     <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="47">
+      <c r="C31" s="36">
         <f>Aporte</f>
-        <v>500</v>
-      </c>
-      <c r="D31" s="48"/>
+        <v>600</v>
+      </c>
+      <c r="D31" s="37"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="53" t="s">
+      <c r="B33" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="51" t="s">
+      <c r="C33" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="53" t="s">
+      <c r="D33" s="29" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="43" t="s">
+      <c r="B34" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="44">
+      <c r="C34" s="22">
         <f>VLOOKUP($C$30&amp;" - "&amp;B34,Planilha2!A3:D20,4,FALSE)</f>
         <v>0.5</v>
       </c>
-      <c r="D34" s="45">
-        <f>C34*$C$31</f>
-        <v>250</v>
+      <c r="D34" s="23">
+        <f t="shared" ref="D34:D39" si="0">C34*$C$31</f>
+        <v>300</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="44">
+      <c r="C35" s="22">
         <f>VLOOKUP($C$30&amp;" - "&amp;B35,Planilha2!A4:D21,4,FALSE)</f>
         <v>0.1</v>
       </c>
-      <c r="D35" s="45">
-        <f>C35*$C$31</f>
-        <v>50</v>
+      <c r="D35" s="23">
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="44">
+      <c r="C36" s="22">
         <f>VLOOKUP($C$30&amp;" - "&amp;B36,Planilha2!A5:D22,4,FALSE)</f>
         <v>0.05</v>
       </c>
-      <c r="D36" s="45">
-        <f>C36*$C$31</f>
-        <v>25</v>
+      <c r="D36" s="23">
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="44">
+      <c r="C37" s="22">
         <f>VLOOKUP($C$30&amp;" - "&amp;B37,Planilha2!A6:D23,4,FALSE)</f>
         <v>0.05</v>
       </c>
-      <c r="D37" s="45">
-        <f>C37*$C$31</f>
-        <v>25</v>
+      <c r="D37" s="23">
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="43" t="s">
+      <c r="B38" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="44">
+      <c r="C38" s="22">
         <f>VLOOKUP($C$30&amp;" - "&amp;B38,Planilha2!A7:D24,4,FALSE)</f>
         <v>0.2</v>
       </c>
-      <c r="D38" s="45">
-        <f>C38*$C$31</f>
-        <v>100</v>
+      <c r="D38" s="23">
+        <f t="shared" si="0"/>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="43" t="s">
+      <c r="B39" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="44">
+      <c r="C39" s="22">
         <f>VLOOKUP($C$30&amp;" - "&amp;B39,Planilha2!A8:D25,4,FALSE)</f>
         <v>0.1</v>
       </c>
-      <c r="D39" s="45">
-        <f>C39*$C$31</f>
-        <v>50</v>
+      <c r="D39" s="23">
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="50" t="s">
+      <c r="B40" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="51"/>
-      <c r="D40" s="52">
+      <c r="C40" s="27"/>
+      <c r="D40" s="28">
         <f>SUM(D34:D39)</f>
-        <v>500</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -2788,8 +2838,8 @@
   <cols>
     <col min="1" max="1" width="29.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="5"/>
+    <col min="3" max="3" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2799,280 +2849,280 @@
       <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="str">
+      <c r="A3" t="str">
         <f>B3&amp;" - "&amp;C3</f>
         <v>Conservador - PAPEL</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="57">
+      <c r="D3" s="31">
         <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="54" t="str">
+      <c r="A4" t="str">
         <f t="shared" ref="A4:A20" si="0">B4&amp;" - "&amp;C4</f>
         <v>Conservador - TIJOLOS</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="57">
+      <c r="D4" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="54" t="str">
+      <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Conservador - HIBRIDOS</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="57">
+      <c r="D5" s="31">
         <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="54" t="str">
+      <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Conservador - FOF'S</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="57">
+      <c r="D6" s="31">
         <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="54" t="str">
+      <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Conservador - DESENVOLVIMENTO</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="57">
+      <c r="D7" s="31">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="55" t="str">
+      <c r="A8" s="30" t="str">
         <f t="shared" si="0"/>
         <v>Conservador - HOTELARIAS</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="59">
+      <c r="D8" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="54" t="str">
+      <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Moderado - PAPEL</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="57">
+      <c r="D9" s="31">
         <v>0.32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="54" t="str">
+      <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>Moderado - TIJOLOS</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="57">
+      <c r="D10" s="31">
         <v>0.4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="54" t="str">
+      <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>Moderado - HIBRIDOS</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="57">
+      <c r="D11" s="31">
         <v>0.08</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="54" t="str">
+      <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>Moderado - FOF'S</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="57">
+      <c r="D12" s="31">
         <v>0.1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="54" t="str">
+      <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>Moderado - DESENVOLVIMENTO</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="57">
+      <c r="D13" s="31">
         <v>0.05</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="55" t="str">
+      <c r="A14" s="30" t="str">
         <f t="shared" si="0"/>
         <v>Moderado - HOTELARIAS</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="58" t="s">
+      <c r="C14" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="59">
+      <c r="D14" s="33">
         <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="54" t="str">
+      <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo - PAPEL</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="57">
+      <c r="D15" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="54" t="str">
+      <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo - TIJOLOS</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="57">
+      <c r="D16" s="31">
         <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="54" t="str">
+      <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo - HIBRIDOS</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="57">
+      <c r="D17" s="31">
         <v>0.05</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="54" t="str">
+      <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo - FOF'S</v>
       </c>
-      <c r="B18" s="54" t="s">
+      <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="57">
+      <c r="D18" s="31">
         <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="54" t="str">
+      <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo - DESENVOLVIMENTO</v>
       </c>
-      <c r="B19" s="54" t="s">
+      <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="56" t="s">
+      <c r="C19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="57">
+      <c r="D19" s="31">
         <v>0.2</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="55" t="str">
+      <c r="A20" s="30" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo - HOTELARIAS</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="58" t="s">
+      <c r="C20" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="59">
+      <c r="D20" s="33">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>